<commit_message>
update BASES.xlsx with blank inputs
</commit_message>
<xml_diff>
--- a/tests/resources/BASES.xlsx
+++ b/tests/resources/BASES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/cameron_pinnegar_education_gov_uk/Documents/Documents/xlcalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpinnegar\OneDrive - Department for Education\Documents\xlcalculator\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{94A8F0F3-6224-4998-8E41-348F3478D04F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD5095B3-EDA2-4D31-BF64-2D7CADBF566F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFC0766-E2A2-4D2F-883D-F525CBA21B73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22597" yWindow="-2400" windowWidth="22695" windowHeight="14595" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dec2" sheetId="1" r:id="rId1"/>
@@ -728,29 +728,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH48"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="F4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="7" width="17.265625" customWidth="1"/>
-    <col min="9" max="10" width="11.19921875" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="10.9296875" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" customWidth="1"/>
-    <col min="16" max="21" width="12.33203125" customWidth="1"/>
-    <col min="23" max="24" width="12.33203125" customWidth="1"/>
-    <col min="25" max="25" width="13.19921875" customWidth="1"/>
-    <col min="26" max="28" width="13.53125" customWidth="1"/>
-    <col min="30" max="30" width="17.46484375" customWidth="1"/>
-    <col min="31" max="31" width="15.3984375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="21" width="12.28515625" customWidth="1"/>
+    <col min="23" max="24" width="12.28515625" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" customWidth="1"/>
+    <col min="26" max="28" width="13.5703125" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -785,7 +785,7 @@
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
     </row>
-    <row r="2" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -862,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -963,7 +963,7 @@
         <v>FFFFFFFFFE</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>FFFFFFFFFD</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>FFFFFFFFFB</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>FFFFFFFFF7</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>FFFFFFFFEF</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>FFFFFFFFDF</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>FFFFFFFFBF</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>FFFFFFFF7F</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>FFFFFFFEFF</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>FFFFFFFDFF</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>FFFFFFFBFF</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>FFFFFFF7FF</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>FFFFFFEFFF</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>FFFFFFDFFF</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>FFFFFFBFFF</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>FFFFFF7FFF</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>FFFFFEFFFF</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>FFFFFDFFFF</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>FFFFFBFFFF</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>FFFFF7FFFF</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>FFFFEFFFFF</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>FFFFDFFFFF</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>FFFFBFFFFF</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>FFFF7FFFFF</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>FFFEFFFFFF</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>FFFDFFFFFF</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>FFFBFFFFFF</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>FFF7FFFFFF</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>FFEFFFFFFF</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>FFDFFFFFFF</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>FFBFFFFFFF</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>FF7FFFFFFF</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>32</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>FEFFFFFFFF</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>33</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>FDFFFFFFFF</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>34</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>FBFFFFFFFF</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>35</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>F7FFFFFFFF</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>36</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>EFFFFFFFFF</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>37</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>DFFFFFFFFF</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>38</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>3777777777</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>39</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>40</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>41</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>42</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>8000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>8000000000</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45</v>
       </c>
@@ -5609,15 +5609,15 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="15.06640625" customWidth="1"/>
+    <col min="1" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>10</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>11</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>111</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1111</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>11111</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>1F</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>111111</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>3F</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010101</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1111111</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>7F</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11111111</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>FF</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>111111111</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>1FF</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1000000000</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>FFFFFFFE00</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1000000001</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>FFFFFFFE01</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1001010101</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>FFFFFFFE55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1111111111</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>FFFFFFFFFF</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10000000000</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -5968,16 +5968,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="15.3984375" customWidth="1"/>
+    <col min="1" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>77</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>3F</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>777</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>1FF</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1000</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7777</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>FFF</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>77777</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>7FFF</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>777777</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>3FFFF</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7777777</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>1FFFFF</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>77777777</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>FFFFFF</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>777777777</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>7FFFFFF</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1000000000</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3777777777</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>1FFFFFFF</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4000000000</v>
       </c>
@@ -6331,7 +6331,7 @@
         <v>FFE0000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4444444444</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>FFE4924924</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7777776777</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>FFFFFFFDFF</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7777777000</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>FFFFFFFE00</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7777777001</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>FFFFFFFE01</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7777777123</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>FFFFFFFE53</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7777777000</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>FFFFFFFE00</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>7777777777</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>FFFFFFFFFF</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10000000000</v>
       </c>
@@ -6481,20 +6481,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1328125" customWidth="1"/>
-    <col min="2" max="4" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="4" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="12.06640625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -6576,7 +6576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>100</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -6780,7 +6780,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>200</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>300</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>1048575</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>16777215</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>268435455</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10000000</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>268435456</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -6934,7 +6934,7 @@
       </c>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -6952,7 +6952,7 @@
       </c>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20000000</v>
       </c>
@@ -6970,7 +6970,7 @@
       </c>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20000001</v>
       </c>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="H29" s="10"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -7006,7 +7006,7 @@
       </c>
       <c r="H30" s="10"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -7024,7 +7024,7 @@
       </c>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1000000000</v>
       </c>
@@ -7042,7 +7042,7 @@
       </c>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -7060,7 +7060,7 @@
       </c>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8000000000</v>
       </c>
@@ -7078,7 +7078,7 @@
       </c>
       <c r="H34" s="10"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>9000000000</v>
       </c>
@@ -7096,7 +7096,7 @@
       </c>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -7132,7 +7132,7 @@
       </c>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="H38" s="10"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -7168,7 +7168,7 @@
       </c>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -7186,7 +7186,7 @@
       </c>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -7204,7 +7204,7 @@
       </c>
       <c r="H41" s="10"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -7222,7 +7222,7 @@
       </c>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -7258,7 +7258,7 @@
       </c>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>10000000000</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -7292,7 +7292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -7340,24 +7340,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5F4525-29BC-435A-8A1E-332B37198F8C}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.796875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" customWidth="1"/>
-    <col min="6" max="6" width="12.1328125" customWidth="1"/>
-    <col min="7" max="7" width="14.265625" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="12.1328125" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>56</v>
       </c>
@@ -7392,7 +7390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -7436,7 +7434,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>10</v>
       </c>
@@ -7480,7 +7478,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>10</v>
       </c>
@@ -7524,7 +7522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>10</v>
       </c>
@@ -7568,7 +7566,7 @@
         <v>020</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>10</v>
       </c>
@@ -7612,7 +7610,7 @@
         <v>0020</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>10</v>
       </c>
@@ -7656,7 +7654,7 @@
         <v>00020</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>10</v>
       </c>
@@ -7700,7 +7698,7 @@
         <v>000020</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>10</v>
       </c>
@@ -7744,7 +7742,7 @@
         <v>0000020</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>10</v>
       </c>
@@ -7788,7 +7786,7 @@
         <v>00000020</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -7832,7 +7830,7 @@
         <v>000000020</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -7876,7 +7874,7 @@
         <v>0000000020</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>10</v>
       </c>
@@ -7920,7 +7918,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>123</v>
       </c>
@@ -7964,7 +7962,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>123</v>
       </c>
@@ -8008,7 +8006,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>123</v>
       </c>
@@ -8052,7 +8050,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>123</v>
       </c>
@@ -8096,7 +8094,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>123</v>
       </c>
@@ -8140,7 +8138,7 @@
         <v>0443</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>123</v>
       </c>
@@ -8184,7 +8182,7 @@
         <v>00443</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>123</v>
       </c>
@@ -8228,7 +8226,7 @@
         <v>000443</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>123</v>
       </c>
@@ -8272,7 +8270,7 @@
         <v>0000443</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>123</v>
       </c>
@@ -8316,7 +8314,7 @@
         <v>00000443</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>123</v>
       </c>
@@ -8360,7 +8358,7 @@
         <v>000000443</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>123</v>
       </c>
@@ -8404,7 +8402,7 @@
         <v>0000000443</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>123</v>
       </c>
@@ -8448,7 +8446,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>-25</v>
       </c>
@@ -8492,7 +8490,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>-25</v>
       </c>
@@ -8536,7 +8534,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <v>-25</v>
       </c>
@@ -8580,7 +8578,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
         <v>-25</v>
       </c>
@@ -8624,7 +8622,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>-25</v>
       </c>
@@ -8668,7 +8666,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
         <v>-25</v>
       </c>
@@ -8712,7 +8710,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
         <v>-25</v>
       </c>
@@ -8756,7 +8754,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>-25</v>
       </c>
@@ -8800,7 +8798,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>-25</v>
       </c>
@@ -8844,7 +8842,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <v>-25</v>
       </c>
@@ -8888,7 +8886,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>-25</v>
       </c>
@@ -8932,7 +8930,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <v>-25</v>
       </c>
@@ -8976,7 +8974,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -9020,7 +9018,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>27</v>
       </c>
@@ -9064,7 +9062,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>27</v>
       </c>
@@ -9108,7 +9106,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>27</v>
       </c>
@@ -9152,7 +9150,7 @@
         <v>016</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>27</v>
       </c>
@@ -9196,7 +9194,7 @@
         <v>0016</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>27</v>
       </c>
@@ -9240,7 +9238,7 @@
         <v>00016</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>27</v>
       </c>
@@ -9284,7 +9282,7 @@
         <v>000016</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>27</v>
       </c>
@@ -9328,7 +9326,7 @@
         <v>0000016</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>27</v>
       </c>
@@ -9372,7 +9370,7 @@
         <v>00000016</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>27</v>
       </c>
@@ -9416,7 +9414,7 @@
         <v>000000016</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>27</v>
       </c>
@@ -9460,7 +9458,7 @@
         <v>0000000016</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>27</v>
       </c>
@@ -9514,25 +9512,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064D80C5-7CD0-482D-B2FD-DC296BB55253}">
   <dimension ref="A1:AO37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="13" width="11.796875" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="27" width="11.33203125" customWidth="1"/>
-    <col min="29" max="29" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="41" width="12.46484375" customWidth="1"/>
+    <col min="2" max="13" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="27" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="41" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -9563,7 +9561,7 @@
       <c r="AN3" s="10"/>
       <c r="AO3" s="10"/>
     </row>
-    <row r="4" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>56</v>
       </c>
@@ -9682,7 +9680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>0</v>
       </c>
@@ -9837,7 +9835,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>1</v>
       </c>
@@ -9992,7 +9990,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>2</v>
       </c>
@@ -10147,7 +10145,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>3</v>
       </c>
@@ -10302,7 +10300,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>-1</v>
       </c>
@@ -10457,7 +10455,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>-2</v>
       </c>
@@ -10612,7 +10610,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>-3</v>
       </c>
@@ -10767,7 +10765,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="12" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -10922,7 +10920,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -11077,7 +11075,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -11232,7 +11230,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>-11</v>
       </c>
@@ -11387,7 +11385,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="16" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>-12</v>
       </c>
@@ -11542,7 +11540,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>-13</v>
       </c>
@@ -11697,7 +11695,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="18" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>101</v>
       </c>
@@ -11852,7 +11850,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>102</v>
       </c>
@@ -12007,7 +12005,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="20" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>103</v>
       </c>
@@ -12162,7 +12160,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="21" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>-101</v>
       </c>
@@ -12317,7 +12315,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="22" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>-102</v>
       </c>
@@ -12472,7 +12470,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>-103</v>
       </c>
@@ -12627,7 +12625,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="24" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>510</v>
       </c>
@@ -12784,7 +12782,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="25" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>511</v>
       </c>
@@ -12941,7 +12939,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="26" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>512</v>
       </c>
@@ -13098,7 +13096,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="27" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>513</v>
       </c>
@@ -13255,7 +13253,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="28" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>-510</v>
       </c>
@@ -13412,7 +13410,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="29" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>-511</v>
       </c>
@@ -13569,7 +13567,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="30" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>-512</v>
       </c>
@@ -13726,7 +13724,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="31" spans="1:41" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>-513</v>
       </c>
@@ -13883,7 +13881,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
@@ -13897,7 +13895,7 @@
       <c r="Z32" s="10"/>
       <c r="AA32" s="10"/>
     </row>
-    <row r="33" spans="16:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="16:27" x14ac:dyDescent="0.2">
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
@@ -13911,7 +13909,7 @@
       <c r="Z33" s="10"/>
       <c r="AA33" s="10"/>
     </row>
-    <row r="34" spans="16:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="16:27" x14ac:dyDescent="0.2">
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
@@ -13925,7 +13923,7 @@
       <c r="Z34" s="10"/>
       <c r="AA34" s="10"/>
     </row>
-    <row r="35" spans="16:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="16:27" x14ac:dyDescent="0.2">
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
@@ -13939,7 +13937,7 @@
       <c r="Z35" s="10"/>
       <c r="AA35" s="10"/>
     </row>
-    <row r="36" spans="16:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="16:27" x14ac:dyDescent="0.2">
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
@@ -13953,7 +13951,7 @@
       <c r="Z36" s="10"/>
       <c r="AA36" s="10"/>
     </row>
-    <row r="37" spans="16:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="16:27" x14ac:dyDescent="0.2">
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
@@ -13975,15 +13973,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6502EA-E4C7-407D-A5DD-F91B4FE71DB5}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
@@ -14021,902 +14019,967 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B2" t="str">
-        <f>BIN2OCT(A2)</f>
+        <f t="shared" ref="B2:B19" si="0">BIN2OCT(A2)</f>
         <v>0</v>
       </c>
       <c r="C2" s="10">
-        <f>BIN2DEC(A2)</f>
+        <f t="shared" ref="C2:C19" si="1">BIN2DEC(A2)</f>
         <v>0</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f>BIN2HEX(A2)</f>
+        <f t="shared" ref="D2:D19" si="2">BIN2HEX(A2)</f>
         <v>0</v>
       </c>
       <c r="E2" s="10" t="str">
-        <f>OCT2BIN(A2)</f>
+        <f t="shared" ref="E2:E19" si="3">OCT2BIN(A2)</f>
         <v>0</v>
       </c>
       <c r="F2" s="10">
-        <f>OCT2DEC(A2)</f>
+        <f t="shared" ref="F2:F19" si="4">OCT2DEC(A2)</f>
         <v>0</v>
       </c>
       <c r="G2" s="10" t="str">
-        <f>OCT2HEX(A2)</f>
+        <f t="shared" ref="G2:G19" si="5">OCT2HEX(A2)</f>
         <v>0</v>
       </c>
       <c r="H2" s="10" t="str">
-        <f>DEC2BIN(A2)</f>
+        <f t="shared" ref="H2:H19" si="6">DEC2BIN(A2)</f>
         <v>0</v>
       </c>
       <c r="I2" s="10" t="str">
-        <f>DEC2OCT(A2)</f>
+        <f t="shared" ref="I2:I19" si="7">DEC2OCT(A2)</f>
         <v>0</v>
       </c>
       <c r="J2" s="10" t="str">
-        <f>DEC2HEX(A2)</f>
+        <f t="shared" ref="J2:J19" si="8">DEC2HEX(A2)</f>
         <v>0</v>
       </c>
       <c r="K2" s="10" t="str">
-        <f>HEX2BIN(A2)</f>
+        <f t="shared" ref="K2:K19" si="9">HEX2BIN(A2)</f>
         <v>0</v>
       </c>
       <c r="L2" s="10" t="str">
-        <f>HEX2OCT(A2)</f>
+        <f t="shared" ref="L2:L19" si="10">HEX2OCT(A2)</f>
         <v>0</v>
       </c>
       <c r="M2" s="10">
-        <f>HEX2DEC(A2)</f>
+        <f t="shared" ref="M2:M19" si="11">HEX2DEC(A2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="B3" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <f t="shared" ref="C3" si="12">BIN2DEC(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="str">
+        <f t="shared" ref="D3" si="13">BIN2HEX(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="str">
+        <f t="shared" ref="E3" si="14">OCT2BIN(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3" si="15">OCT2DEC(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="10" t="str">
+        <f t="shared" ref="G3" si="16">OCT2HEX(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="10" t="e">
+        <f t="shared" ref="H3" si="17">DEC2BIN(A3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" s="10" t="e">
+        <f t="shared" ref="I3" si="18">DEC2OCT(A3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="10" t="e">
+        <f t="shared" ref="J3" si="19">DEC2HEX(A3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="10" t="str">
+        <f t="shared" ref="K3" si="20">HEX2BIN(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="10" t="str">
+        <f t="shared" ref="L3" si="21">HEX2OCT(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="10">
+        <f t="shared" ref="M3" si="22">HEX2DEC(A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="10" t="e">
-        <f>BIN2OCT(A3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C3" s="10" t="e">
-        <f>BIN2DEC(A3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D3" s="10" t="e">
-        <f>BIN2HEX(A3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E3" s="10" t="e">
-        <f>OCT2BIN(A3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F3" s="10" t="e">
-        <f>OCT2DEC(A3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G3" s="10" t="e">
-        <f>OCT2HEX(A3)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H3" s="10" t="e">
-        <f>DEC2BIN(A3)</f>
+      <c r="B4" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C4" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D4" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E4" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F4" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G4" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H4" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I3" s="10" t="e">
-        <f>DEC2OCT(A3)</f>
+      <c r="I4" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J3" s="10" t="e">
-        <f>DEC2HEX(A3)</f>
+      <c r="J4" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K3" s="10" t="str">
-        <f>HEX2BIN(A3)</f>
+      <c r="K4" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1010</v>
       </c>
-      <c r="L3" s="10" t="str">
-        <f>HEX2OCT(A3)</f>
+      <c r="L4" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="M3" s="10">
-        <f>HEX2DEC(A3)</f>
+      <c r="M4" s="10">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="10" t="e">
-        <f>BIN2OCT(A4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C4" s="10" t="e">
-        <f>BIN2DEC(A4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D4" s="10" t="e">
-        <f>BIN2HEX(A4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E4" s="10" t="e">
-        <f>OCT2BIN(A4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F4" s="10" t="e">
-        <f>OCT2DEC(A4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G4" s="10" t="e">
-        <f>OCT2HEX(A4)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H4" s="10" t="e">
-        <f>DEC2BIN(A4)</f>
+      <c r="B5" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C5" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D5" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E5" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F5" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G5" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H5" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I4" s="10" t="e">
-        <f>DEC2OCT(A4)</f>
+      <c r="I5" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J4" s="10" t="e">
-        <f>DEC2HEX(A4)</f>
+      <c r="J5" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K4" s="10" t="str">
-        <f>HEX2BIN(A4)</f>
+      <c r="K5" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1010</v>
       </c>
-      <c r="L4" s="10" t="str">
-        <f>HEX2OCT(A4)</f>
+      <c r="L5" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="M4" s="10">
-        <f>HEX2DEC(A4)</f>
+      <c r="M5" s="10">
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10" t="e">
-        <f>BIN2OCT(A5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C5" s="10" t="e">
-        <f>BIN2DEC(A5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D5" s="10" t="e">
-        <f>BIN2HEX(A5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E5" s="10" t="e">
-        <f>OCT2BIN(A5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F5" s="10" t="e">
-        <f>OCT2DEC(A5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G5" s="10" t="e">
-        <f>OCT2HEX(A5)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H5" s="10" t="e">
-        <f>DEC2BIN(A5)</f>
+      <c r="B6" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C6" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D6" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E6" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F6" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G6" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H6" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I5" s="10" t="e">
-        <f>DEC2OCT(A5)</f>
+      <c r="I6" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J5" s="10" t="e">
-        <f>DEC2HEX(A5)</f>
+      <c r="J6" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K5" s="10" t="str">
-        <f>HEX2BIN(A5)</f>
+      <c r="K6" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1011</v>
       </c>
-      <c r="L5" s="10" t="str">
-        <f>HEX2OCT(A5)</f>
+      <c r="L6" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
-      <c r="M5" s="10">
-        <f>HEX2DEC(A5)</f>
+      <c r="M6" s="10">
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="10" t="e">
-        <f>BIN2OCT(A6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C6" s="10" t="e">
-        <f>BIN2DEC(A6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D6" s="10" t="e">
-        <f>BIN2HEX(A6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E6" s="10" t="e">
-        <f>OCT2BIN(A6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F6" s="10" t="e">
-        <f>OCT2DEC(A6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G6" s="10" t="e">
-        <f>OCT2HEX(A6)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H6" s="10" t="e">
-        <f>DEC2BIN(A6)</f>
+      <c r="B7" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C7" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D7" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E7" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F7" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G7" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H7" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I6" s="10" t="e">
-        <f>DEC2OCT(A6)</f>
+      <c r="I7" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J6" s="10" t="e">
-        <f>DEC2HEX(A6)</f>
+      <c r="J7" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K6" s="10" t="str">
-        <f>HEX2BIN(A6)</f>
+      <c r="K7" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1011</v>
       </c>
-      <c r="L6" s="10" t="str">
-        <f>HEX2OCT(A6)</f>
+      <c r="L7" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
-      <c r="M6" s="10">
-        <f>HEX2DEC(A6)</f>
+      <c r="M7" s="10">
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="e">
-        <f>BIN2OCT(A7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C7" s="10" t="e">
-        <f>BIN2DEC(A7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D7" s="10" t="e">
-        <f>BIN2HEX(A7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E7" s="10" t="e">
-        <f>OCT2BIN(A7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F7" s="10" t="e">
-        <f>OCT2DEC(A7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G7" s="10" t="e">
-        <f>OCT2HEX(A7)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H7" s="10" t="e">
-        <f>DEC2BIN(A7)</f>
+      <c r="B8" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C8" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D8" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E8" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F8" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G8" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H8" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I7" s="10" t="e">
-        <f>DEC2OCT(A7)</f>
+      <c r="I8" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J7" s="10" t="e">
-        <f>DEC2HEX(A7)</f>
+      <c r="J8" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K7" s="10" t="str">
-        <f>HEX2BIN(A7)</f>
+      <c r="K8" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1100</v>
       </c>
-      <c r="L7" s="10" t="str">
-        <f>HEX2OCT(A7)</f>
+      <c r="L8" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="M7" s="10">
-        <f>HEX2DEC(A7)</f>
+      <c r="M8" s="10">
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="10" t="e">
-        <f>BIN2OCT(A8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C8" s="10" t="e">
-        <f>BIN2DEC(A8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D8" s="10" t="e">
-        <f>BIN2HEX(A8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E8" s="10" t="e">
-        <f>OCT2BIN(A8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F8" s="10" t="e">
-        <f>OCT2DEC(A8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G8" s="10" t="e">
-        <f>OCT2HEX(A8)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H8" s="10" t="e">
-        <f>DEC2BIN(A8)</f>
+      <c r="B9" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C9" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D9" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E9" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F9" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G9" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H9" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I8" s="10" t="e">
-        <f>DEC2OCT(A8)</f>
+      <c r="I9" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J8" s="10" t="e">
-        <f>DEC2HEX(A8)</f>
+      <c r="J9" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K8" s="10" t="str">
-        <f>HEX2BIN(A8)</f>
+      <c r="K9" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1100</v>
       </c>
-      <c r="L8" s="10" t="str">
-        <f>HEX2OCT(A8)</f>
+      <c r="L9" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="M8" s="10">
-        <f>HEX2DEC(A8)</f>
+      <c r="M9" s="10">
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="10" t="e">
-        <f>BIN2OCT(A9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C9" s="10" t="e">
-        <f>BIN2DEC(A9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D9" s="10" t="e">
-        <f>BIN2HEX(A9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E9" s="10" t="e">
-        <f>OCT2BIN(A9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F9" s="10" t="e">
-        <f>OCT2DEC(A9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G9" s="10" t="e">
-        <f>OCT2HEX(A9)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H9" s="10" t="e">
-        <f>DEC2BIN(A9)</f>
+      <c r="B10" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C10" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D10" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E10" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F10" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G10" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H10" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I9" s="10" t="e">
-        <f>DEC2OCT(A9)</f>
+      <c r="I10" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J9" s="10" t="e">
-        <f>DEC2HEX(A9)</f>
+      <c r="J10" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K9" s="10" t="str">
-        <f>HEX2BIN(A9)</f>
+      <c r="K10" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1101</v>
       </c>
-      <c r="L9" s="10" t="str">
-        <f>HEX2OCT(A9)</f>
+      <c r="L10" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
-      <c r="M9" s="10">
-        <f>HEX2DEC(A9)</f>
+      <c r="M10" s="10">
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="10" t="e">
-        <f>BIN2OCT(A10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C10" s="10" t="e">
-        <f>BIN2DEC(A10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D10" s="10" t="e">
-        <f>BIN2HEX(A10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E10" s="10" t="e">
-        <f>OCT2BIN(A10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" s="10" t="e">
-        <f>OCT2DEC(A10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G10" s="10" t="e">
-        <f>OCT2HEX(A10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H10" s="10" t="e">
-        <f>DEC2BIN(A10)</f>
+      <c r="B11" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C11" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D11" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E11" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F11" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G11" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H11" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I10" s="10" t="e">
-        <f>DEC2OCT(A10)</f>
+      <c r="I11" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J10" s="10" t="e">
-        <f>DEC2HEX(A10)</f>
+      <c r="J11" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K10" s="10" t="str">
-        <f>HEX2BIN(A10)</f>
+      <c r="K11" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1101</v>
       </c>
-      <c r="L10" s="10" t="str">
-        <f>HEX2OCT(A10)</f>
+      <c r="L11" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
-      <c r="M10" s="10">
-        <f>HEX2DEC(A10)</f>
+      <c r="M11" s="10">
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="10" t="e">
-        <f>BIN2OCT(A11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C11" s="10" t="e">
-        <f>BIN2DEC(A11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D11" s="10" t="e">
-        <f>BIN2HEX(A11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E11" s="10" t="e">
-        <f>OCT2BIN(A11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F11" s="10" t="e">
-        <f>OCT2DEC(A11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G11" s="10" t="e">
-        <f>OCT2HEX(A11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H11" s="10" t="e">
-        <f>DEC2BIN(A11)</f>
+      <c r="B12" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C12" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D12" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E12" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F12" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G12" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H12" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I11" s="10" t="e">
-        <f>DEC2OCT(A11)</f>
+      <c r="I12" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J11" s="10" t="e">
-        <f>DEC2HEX(A11)</f>
+      <c r="J12" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K11" s="10" t="str">
-        <f>HEX2BIN(A11)</f>
+      <c r="K12" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1110</v>
       </c>
-      <c r="L11" s="10" t="str">
-        <f>HEX2OCT(A11)</f>
+      <c r="L12" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
-      <c r="M11" s="10">
-        <f>HEX2DEC(A11)</f>
+      <c r="M12" s="10">
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="10" t="e">
-        <f>BIN2OCT(A12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C12" s="10" t="e">
-        <f>BIN2DEC(A12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D12" s="10" t="e">
-        <f>BIN2HEX(A12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E12" s="10" t="e">
-        <f>OCT2BIN(A12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F12" s="10" t="e">
-        <f>OCT2DEC(A12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G12" s="10" t="e">
-        <f>OCT2HEX(A12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H12" s="10" t="e">
-        <f>DEC2BIN(A12)</f>
+      <c r="B13" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C13" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D13" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E13" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F13" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G13" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H13" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I12" s="10" t="e">
-        <f>DEC2OCT(A12)</f>
+      <c r="I13" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J12" s="10" t="e">
-        <f>DEC2HEX(A12)</f>
+      <c r="J13" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K12" s="10" t="str">
-        <f>HEX2BIN(A12)</f>
+      <c r="K13" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1110</v>
       </c>
-      <c r="L12" s="10" t="str">
-        <f>HEX2OCT(A12)</f>
+      <c r="L13" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
-      <c r="M12" s="10">
-        <f>HEX2DEC(A12)</f>
+      <c r="M13" s="10">
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="10" t="e">
-        <f>BIN2OCT(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C13" s="10" t="e">
-        <f>BIN2DEC(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D13" s="10" t="e">
-        <f>BIN2HEX(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E13" s="10" t="e">
-        <f>OCT2BIN(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F13" s="10" t="e">
-        <f>OCT2DEC(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G13" s="10" t="e">
-        <f>OCT2HEX(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H13" s="10" t="e">
-        <f>DEC2BIN(A13)</f>
+      <c r="B14" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C14" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D14" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E14" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F14" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G14" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H14" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I13" s="10" t="e">
-        <f>DEC2OCT(A13)</f>
+      <c r="I14" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J13" s="10" t="e">
-        <f>DEC2HEX(A13)</f>
+      <c r="J14" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K13" s="10" t="str">
-        <f>HEX2BIN(A13)</f>
+      <c r="K14" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1111</v>
       </c>
-      <c r="L13" s="10" t="str">
-        <f>HEX2OCT(A13)</f>
+      <c r="L14" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
-      <c r="M13" s="10">
-        <f>HEX2DEC(A13)</f>
+      <c r="M14" s="10">
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="Q14">
+        <v>110</v>
+      </c>
+      <c r="R14" t="str">
+        <f>BIN2HEX(Q14,Q15)</f>
+        <v>00006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="10" t="e">
-        <f>BIN2OCT(A14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C14" s="10" t="e">
-        <f>BIN2DEC(A14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D14" s="10" t="e">
-        <f>BIN2HEX(A14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E14" s="10" t="e">
-        <f>OCT2BIN(A14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F14" s="10" t="e">
-        <f>OCT2DEC(A14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G14" s="10" t="e">
-        <f>OCT2HEX(A14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H14" s="10" t="e">
-        <f>DEC2BIN(A14)</f>
+      <c r="B15" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C15" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D15" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E15" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F15" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G15" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H15" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I14" s="10" t="e">
-        <f>DEC2OCT(A14)</f>
+      <c r="I15" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J14" s="10" t="e">
-        <f>DEC2HEX(A14)</f>
+      <c r="J15" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K14" s="10" t="str">
-        <f>HEX2BIN(A14)</f>
+      <c r="K15" s="10" t="str">
+        <f t="shared" si="9"/>
         <v>1111</v>
       </c>
-      <c r="L14" s="10" t="str">
-        <f>HEX2OCT(A14)</f>
+      <c r="L15" s="10" t="str">
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
-      <c r="M14" s="10">
-        <f>HEX2DEC(A14)</f>
+      <c r="M15" s="10">
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="Q15" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10" t="e">
-        <f>BIN2OCT(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C15" s="10" t="e">
-        <f>BIN2DEC(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D15" s="10" t="e">
-        <f>BIN2HEX(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E15" s="10" t="e">
-        <f>OCT2BIN(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F15" s="10" t="e">
-        <f>OCT2DEC(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G15" s="10" t="e">
-        <f>OCT2HEX(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H15" s="10" t="e">
-        <f>DEC2BIN(A15)</f>
+      <c r="B16" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C16" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D16" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E16" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F16" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G16" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H16" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I15" s="10" t="e">
-        <f>DEC2OCT(A15)</f>
+      <c r="I16" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J15" s="10" t="e">
-        <f>DEC2HEX(A15)</f>
+      <c r="J16" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K15" s="10" t="e">
-        <f>HEX2BIN(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L15" s="10" t="e">
-        <f>HEX2OCT(A15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M15" s="10" t="e">
-        <f>HEX2DEC(A15)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="K16" s="10" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L16" s="10" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M16" s="10" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="10" t="e">
-        <f>BIN2OCT(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C16" s="10" t="e">
-        <f>BIN2DEC(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D16" s="10" t="e">
-        <f>BIN2HEX(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E16" s="10" t="e">
-        <f>OCT2BIN(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F16" s="10" t="e">
-        <f>OCT2DEC(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G16" s="10" t="e">
-        <f>OCT2HEX(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H16" s="10" t="e">
-        <f>DEC2BIN(A16)</f>
+      <c r="B17" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C17" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D17" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E17" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F17" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G17" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H17" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I16" s="10" t="e">
-        <f>DEC2OCT(A16)</f>
+      <c r="I17" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J16" s="10" t="e">
-        <f>DEC2HEX(A16)</f>
+      <c r="J17" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K16" s="10" t="e">
-        <f>HEX2BIN(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L16" s="10" t="e">
-        <f>HEX2OCT(A16)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M16" s="10" t="e">
-        <f>HEX2DEC(A16)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="str">
+      <c r="K17" s="10" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L17" s="10" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M17" s="10" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
         <f>"-A"</f>
         <v>-A</v>
       </c>
-      <c r="B17" s="10" t="e">
-        <f>BIN2OCT(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C17" s="10" t="e">
-        <f>BIN2DEC(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D17" s="10" t="e">
-        <f>BIN2HEX(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E17" s="10" t="e">
-        <f>OCT2BIN(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F17" s="10" t="e">
-        <f>OCT2DEC(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G17" s="10" t="e">
-        <f>OCT2HEX(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H17" s="10" t="e">
-        <f>DEC2BIN(A17)</f>
+      <c r="B18" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C18" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D18" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E18" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F18" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G18" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H18" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I17" s="10" t="e">
-        <f>DEC2OCT(A17)</f>
+      <c r="I18" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J17" s="10" t="e">
-        <f>DEC2HEX(A17)</f>
+      <c r="J18" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K17" s="10" t="e">
-        <f>HEX2BIN(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L17" s="10" t="e">
-        <f>HEX2OCT(A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M17" s="10" t="e">
-        <f>HEX2DEC(A17)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="K18" s="10" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L18" s="10" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M18" s="10" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="10" t="e">
-        <f>BIN2OCT(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C18" s="10" t="e">
-        <f>BIN2DEC(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="D18" s="10" t="e">
-        <f>BIN2HEX(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E18" s="10" t="e">
-        <f>OCT2BIN(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F18" s="10" t="e">
-        <f>OCT2DEC(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G18" s="10" t="e">
-        <f>OCT2HEX(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H18" s="10" t="e">
-        <f>DEC2BIN(A18)</f>
+      <c r="B19" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C19" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D19" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="E19" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F19" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G19" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H19" s="10" t="e">
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I18" s="10" t="e">
-        <f>DEC2OCT(A18)</f>
+      <c r="I19" s="10" t="e">
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J18" s="10" t="e">
-        <f>DEC2HEX(A18)</f>
+      <c r="J19" s="10" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K18" s="10" t="e">
-        <f>HEX2BIN(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L18" s="10" t="e">
-        <f>HEX2OCT(A18)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M18" s="10" t="e">
-        <f>HEX2DEC(A18)</f>
+      <c r="K19" s="10" t="e">
+        <f t="shared" si="9"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L19" s="10" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M19" s="10" t="e">
+        <f t="shared" si="11"/>
         <v>#NUM!</v>
       </c>
     </row>

</xml_diff>